<commit_message>
tablas para que se den  formato en ppt
</commit_message>
<xml_diff>
--- a/drafts/parametros_final_ma.xlsx
+++ b/drafts/parametros_final_ma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/1thaliaespana1/Documents/Semestre II/ambientes/sandbox_R/final_met_analit_mcd/drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D14635CE-C3E0-234A-8F95-FD56E5E6E056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD67440C-4556-A845-A6B0-AB803947DEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{B019F1D4-062C-D64F-9BA9-ED98B92B24C6}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{B019F1D4-062C-D64F-9BA9-ED98B92B24C6}"/>
   </bookViews>
   <sheets>
     <sheet name="model1" sheetId="2" r:id="rId1"/>
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -174,7 +174,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E158BE2-8FB9-3647-9133-8CEEFDB3F35A}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,25 +704,25 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10">
         <v>0.98</v>
       </c>
-      <c r="C10" s="11">
-        <v>0.37</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.37</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="C10">
+        <v>0.37</v>
+      </c>
+      <c r="D10">
+        <v>0.37</v>
+      </c>
+      <c r="E10">
         <v>1.56</v>
       </c>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>4202.2</v>
       </c>
     </row>
@@ -759,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E7DE59-C0BA-B049-8055-8DE3550924B7}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>